<commit_message>
adding trade-off summary sheet
</commit_message>
<xml_diff>
--- a/01-Analizy/Trade_off_mp/output_summary.xlsx
+++ b/01-Analizy/Trade_off_mp/output_summary.xlsx
@@ -5,23 +5,84 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\Studia\Napedy_kosmiczne\01-Analizy\Trade_off_mp\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\Studia\Napedy_kosmiczne\01-Analizy\Trade_off_mp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AE1B00-AABB-4BDA-9933-9D2B160844B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9950D9-2DEE-48D2-AF25-29B02328876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>Alternatywy</t>
+  </si>
+  <si>
+    <t>Kryteria</t>
+  </si>
+  <si>
+    <t>Dostępność- 0.8</t>
+  </si>
+  <si>
+    <t>Osiągi- 0.6</t>
+  </si>
+  <si>
+    <t>Użytkowość- 0.3</t>
+  </si>
+  <si>
+    <t>Stopień przebadania- 0.5</t>
+  </si>
+  <si>
+    <t>Metanol</t>
+  </si>
+  <si>
+    <t>Etanol</t>
+  </si>
+  <si>
+    <t>Amoniak</t>
+  </si>
+  <si>
+    <t>Propan</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>H2O2</t>
+  </si>
+  <si>
+    <t>N2O</t>
+  </si>
+  <si>
+    <t>Ocena</t>
+  </si>
+  <si>
+    <t>Toksyczność- 1.0</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -51,12 +112,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -337,14 +441,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="2">
+        <f>1*C3+0.8*D3+0.6*E3+0.3*F3+0.5*G3</f>
+        <v>1.9900000000000002</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2">
+        <f>1*J3+0.8*K3+0.6*L3+0.3*M3+0.5*N3</f>
+        <v>2.4699999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H7" si="0">1*C4+0.8*D4+0.6*E4+0.3*F4+0.5*G4</f>
+        <v>2.33</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <f>1*J4+0.8*K4+0.6*L4+0.3*M4+0.5*N4</f>
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>2.92</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="O1:O2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>